<commit_message>
feat: invocacion a buildCredentials end of form o file
</commit_message>
<xml_diff>
--- a/src/test/resources/files/survey_example.xlsx
+++ b/src/test/resources/files/survey_example.xlsx
@@ -447,10 +447,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I33" activeCellId="0" sqref="33:33"/>
+      <selection pane="bottomRight" activeCell="I33" activeCellId="0" sqref="I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.12890625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.13671875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="0" width="8.82"/>

</xml_diff>

<commit_message>
fix: try-catch and simple function refactor
</commit_message>
<xml_diff>
--- a/src/test/resources/files/survey_example.xlsx
+++ b/src/test/resources/files/survey_example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="74">
   <si>
     <t xml:space="preserve">AREA</t>
   </si>
@@ -239,6 +239,9 @@
   </si>
   <si>
     <t xml:space="preserve">DNI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evaluacin_Socioeconmica1580823537773 – 99</t>
   </si>
 </sst>
 </file>
@@ -447,14 +450,14 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I33" activeCellId="0" sqref="I33"/>
+      <selection pane="bottomRight" activeCell="H35" activeCellId="0" sqref="H35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.13671875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.14453125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="0" width="8.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="34.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="40.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.55"/>
@@ -2149,6 +2152,59 @@
         <v>71</v>
       </c>
       <c r="Q32" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="I34" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J34" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="K34" s="0" t="n">
+        <v>5552007</v>
+      </c>
+      <c r="L34" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M34" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="N34" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="O34" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="P34" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q34" s="0" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: create credentials and persons and check if those exists
</commit_message>
<xml_diff>
--- a/src/test/resources/files/survey_example.xlsx
+++ b/src/test/resources/files/survey_example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="74">
   <si>
     <t xml:space="preserve">AREA</t>
   </si>
@@ -239,6 +239,9 @@
   </si>
   <si>
     <t xml:space="preserve">Evaluacin_Socioeconmica1580823537773 – 99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27/03/2099</t>
   </si>
 </sst>
 </file>
@@ -440,15 +443,15 @@
   </sheetPr>
   <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q3" activeCellId="0" sqref="Q3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J34" activeCellId="0" sqref="J34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.93"/>
@@ -461,9 +464,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="21.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="19.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="24.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="27.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="34.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="15.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="27.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="34.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="15.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2233,7 +2236,7 @@
         <v>22</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="K34" s="3" t="n">
         <v>5552007</v>

</xml_diff>

<commit_message>
fix: added totalProcessedForms to fileUpload response
</commit_message>
<xml_diff>
--- a/src/test/resources/files/survey_example.xlsx
+++ b/src/test/resources/files/survey_example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="73">
   <si>
     <t xml:space="preserve">AREA</t>
   </si>
@@ -239,9 +239,6 @@
   </si>
   <si>
     <t xml:space="preserve">Evaluacin_Socioeconmica1580823537773 – 99</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27/03/2099</t>
   </si>
 </sst>
 </file>
@@ -444,10 +441,10 @@
   <dimension ref="A1:R34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J34" activeCellId="0" sqref="J34"/>
+      <selection pane="topLeft" activeCell="J35" activeCellId="0" sqref="J35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.63"/>
@@ -465,7 +462,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="19.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="24.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="27.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="34.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="34.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="15.34"/>
   </cols>
   <sheetData>
@@ -2236,7 +2233,7 @@
         <v>22</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>73</v>
+        <v>23</v>
       </c>
       <c r="K34" s="3" t="n">
         <v>5552007</v>

</xml_diff>

<commit_message>
fix: revisar form antes de crear credenciales
</commit_message>
<xml_diff>
--- a/src/test/resources/files/survey_example.xlsx
+++ b/src/test/resources/files/survey_example.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="75">
   <si>
     <t xml:space="preserve">AREA</t>
   </si>
@@ -236,6 +236,12 @@
   </si>
   <si>
     <t xml:space="preserve">DNI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M</t>
   </si>
   <si>
     <t xml:space="preserve">Evaluacin_Socioeconmica1580823537773 – 99</t>
@@ -441,10 +447,10 @@
   <dimension ref="A1:R34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J35" activeCellId="0" sqref="J35"/>
+      <selection pane="topLeft" activeCell="H35" activeCellId="0" sqref="H35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.63"/>
@@ -2185,23 +2191,57 @@
       <c r="R32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
-      <c r="O33" s="3"/>
-      <c r="P33" s="3"/>
-      <c r="Q33" s="3"/>
+      <c r="A33" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K33" s="3" t="n">
+        <v>5552007</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M33" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N33" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O33" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P33" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q33" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="R33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2227,7 +2267,7 @@
         <v>20</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I34" s="3" t="s">
         <v>22</v>

</xml_diff>